<commit_message>
Create persons based on form upload
</commit_message>
<xml_diff>
--- a/myproject/static/media/sample_dsc.xlsx
+++ b/myproject/static/media/sample_dsc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaitanya/Coding/Projects/DSC_Hackathon/myproject/static/media/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25D1981E-C469-44B1-849D-E0968AE76180}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CC9C94-C31D-0F45-98A8-57C5D8FF7389}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2280" yWindow="2280" windowWidth="14400" windowHeight="7360" xr2:uid="{B9C19D03-F512-4994-988A-3FA5B7C4EF37}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Team</t>
   </si>
   <si>
-    <t xml:space="preserve">Email </t>
-  </si>
-  <si>
     <t>Birthday</t>
   </si>
   <si>
@@ -72,6 +69,9 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -438,16 +438,16 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="19.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,24 +455,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="D2">
         <v>81231233</v>
@@ -481,15 +481,15 @@
         <v>34943</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D3">
         <v>84001400</v>
@@ -498,13 +498,14 @@
         <v>29301</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C4" s="1"/>
       <c r="D4">
         <v>91231234</v>
       </c>

</xml_diff>

<commit_message>
Fix date parsing for excel
</commit_message>
<xml_diff>
--- a/myproject/static/media/sample_dsc.xlsx
+++ b/myproject/static/media/sample_dsc.xlsx
@@ -466,25 +466,25 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mark Brown</t>
+          <t>Sara Macias</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Decentralized interactive migration</t>
+          <t>Phased multi-state extranet</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>johnsontiffany@butler.com</t>
+          <t>dcollins@green.net</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>85207400</v>
+        <v>85071638</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1978-05-10</t>
+          <t>21/03/1990</t>
         </is>
       </c>
     </row>
@@ -494,25 +494,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Katelyn Hall</t>
+          <t>Beth Little</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Operative needs-based process improvement</t>
+          <t>Stand-alone responsive throughput</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>guerrerolaurie@gmail.com</t>
+          <t>tromero@gmail.com</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>88913686</v>
+        <v>81578324</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2011-07-12</t>
+          <t>21/02/1983</t>
         </is>
       </c>
     </row>
@@ -522,25 +522,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jose Mendoza</t>
+          <t>Michelle Smith</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Reverse-engineered value-added benchmark</t>
+          <t>Expanded fault-tolerant secured line</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>lesliedaniels@yahoo.com</t>
+          <t>victoria56@hotmail.com</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>81974634</v>
+        <v>87343230</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1974-12-17</t>
+          <t>05/11/1972</t>
         </is>
       </c>
     </row>
@@ -550,25 +550,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Casey Rodriguez</t>
+          <t>Brian Lee</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Public-key dynamic alliance</t>
+          <t>Devolved intangible archive</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>nicholasmontgomery@fields.com</t>
+          <t>ryan42@yahoo.com</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>85420147</v>
+        <v>87592181</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1997-11-10</t>
+          <t>02/02/2021</t>
         </is>
       </c>
     </row>
@@ -578,25 +578,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>James Mitchell</t>
+          <t>Brett Fleming</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Quality-focused reciprocal moratorium</t>
+          <t>Implemented multi-state hub</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>lchambers@gmail.com</t>
+          <t>andre69@hotmail.com</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>86761710</v>
+        <v>80657926</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2000-10-21</t>
+          <t>21/09/1973</t>
         </is>
       </c>
     </row>
@@ -606,25 +606,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kathryn Sullivan</t>
+          <t>Mitchell Hill</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Grass-roots content-based approach</t>
+          <t>Up-sized multi-state concept</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>catherinecarter@yahoo.com</t>
+          <t>geraldtodd@yahoo.com</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>89045224</v>
+        <v>80192383</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2011-12-22</t>
+          <t>21/02/2002</t>
         </is>
       </c>
     </row>
@@ -634,25 +634,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Michael Arnold</t>
+          <t>Laura Andrews</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Object-based 24/7 migration</t>
+          <t>Optional maximized benchmark</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>brittanygreen@johnson.com</t>
+          <t>wandaallen@smith.net</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>88943622</v>
+        <v>82100473</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2013-06-18</t>
+          <t>19/05/2011</t>
         </is>
       </c>
     </row>
@@ -662,25 +662,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Eugene Lewis</t>
+          <t>Rachel Lowe</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Profit-focused next generation ability</t>
+          <t>Assimilated discrete protocol</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>nrobinson@green.biz</t>
+          <t>nicholsashlee@ward.net</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>82867527</v>
+        <v>87188203</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2011-04-18</t>
+          <t>09/02/2002</t>
         </is>
       </c>
     </row>
@@ -690,25 +690,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Renee Johnson</t>
+          <t>Heather Lin DDS</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Phased bi-directional toolset</t>
+          <t>Seamless executive time-frame</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>moorecharles@taylor.info</t>
+          <t>obrady@hotmail.com</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>88391174</v>
+        <v>81061314</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1998-05-18</t>
+          <t>31/01/1972</t>
         </is>
       </c>
     </row>
@@ -718,25 +718,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>David Williams</t>
+          <t>Linda Burns</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Profound asynchronous protocol</t>
+          <t>Face-to-face methodical methodology</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>ujenkins@cline.com</t>
+          <t>ynavarro@yahoo.com</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>81403404</v>
+        <v>85208569</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1981-12-25</t>
+          <t>02/03/1978</t>
         </is>
       </c>
     </row>
@@ -746,25 +746,25 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Jeremiah Henson</t>
+          <t>Jessica Heath</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Decentralized needs-based knowledgebase</t>
+          <t>Reduced maximized standardization</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>lloydchristopher@hotmail.com</t>
+          <t>gweber@gmail.com</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>89018934</v>
+        <v>81899424</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2020-03-24</t>
+          <t>02/10/1993</t>
         </is>
       </c>
     </row>
@@ -774,25 +774,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Trevor Duncan</t>
+          <t>Erika Garcia</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Realigned zero tolerance hub</t>
+          <t>Focused 5thgeneration open architecture</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>agonzalez@alexander-arroyo.org</t>
+          <t>derrick47@yahoo.com</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>88402089</v>
+        <v>85843326</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2010-11-20</t>
+          <t>19/04/2012</t>
         </is>
       </c>
     </row>
@@ -802,25 +802,25 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Kenneth Nelson</t>
+          <t>Kevin Clark</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Monitored contextually-based secured line</t>
+          <t>Centralized didactic software</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>colemanjennifer@hotmail.com</t>
+          <t>qbaird@gmail.com</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>88268596</v>
+        <v>84420696</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2014-06-29</t>
+          <t>30/07/2008</t>
         </is>
       </c>
     </row>
@@ -830,25 +830,25 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Jared Hernandez</t>
+          <t>Michael Chang</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Customer-focused motivating help-desk</t>
+          <t>Inverse multimedia workforce</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>jennifer36@gmail.com</t>
+          <t>powersjennifer@flowers.com</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>86789727</v>
+        <v>89749866</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2012-11-02</t>
+          <t>15/11/1999</t>
         </is>
       </c>
     </row>
@@ -858,25 +858,25 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Robert Klein</t>
+          <t>Troy Mitchell</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Upgradable mission-critical ability</t>
+          <t>Front-line uniform success</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>kellyrose@gmail.com</t>
+          <t>james82@hotmail.com</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>87837647</v>
+        <v>86916974</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2012-06-24</t>
+          <t>05/06/2010</t>
         </is>
       </c>
     </row>
@@ -886,25 +886,25 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Katie Valdez</t>
+          <t>Frank Price</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Diverse leadingedge process improvement</t>
+          <t>Open-architected well-modulated firmware</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>davidpierce@yahoo.com</t>
+          <t>joneschristina@hart.com</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>80775207</v>
+        <v>87195730</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2000-10-30</t>
+          <t>07/07/1985</t>
         </is>
       </c>
     </row>
@@ -914,25 +914,25 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Jonathan Mccarty</t>
+          <t>Kenneth Boone</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Business-focused multi-state protocol</t>
+          <t>Versatile regional portal</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>christopher28@bell.biz</t>
+          <t>donaldwhite@richmond-palmer.com</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>81040106</v>
+        <v>86203079</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>1990-09-11</t>
+          <t>16/05/1991</t>
         </is>
       </c>
     </row>
@@ -942,25 +942,25 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Holly Wise</t>
+          <t>Danielle Diaz</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Realigned client-server installation</t>
+          <t>Polarized bottom-line concept</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>camerondavis@hotmail.com</t>
+          <t>bvillanueva@washington.biz</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>83448869</v>
+        <v>85329479</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2007-09-11</t>
+          <t>14/01/2015</t>
         </is>
       </c>
     </row>
@@ -970,25 +970,25 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Taylor Noble</t>
+          <t>Matthew Morrison</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Organized human-resource functionalities</t>
+          <t>Function-based web-enabled parallelism</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>sarah86@patterson.info</t>
+          <t>scottmitchell@gmail.com</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>82674415</v>
+        <v>84885981</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2004-04-19</t>
+          <t>10/09/1980</t>
         </is>
       </c>
     </row>
@@ -998,25 +998,25 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Robert Brooks</t>
+          <t>William Lawson</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Exclusive optimal strategy</t>
+          <t>Exclusive modular framework</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>hardingdiane@butler.net</t>
+          <t>khudson@mcdonald-nelson.info</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>88700835</v>
+        <v>86936353</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2010-01-13</t>
+          <t>21/10/2015</t>
         </is>
       </c>
     </row>
@@ -1026,25 +1026,25 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Carl Burns</t>
+          <t>William Johns</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Versatile tangible attitude</t>
+          <t>Reactive clear-thinking framework</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>williamsandrew@yahoo.com</t>
+          <t>charles54@gonzalez.com</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>80210511</v>
+        <v>84929032</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1991-10-16</t>
+          <t>14/05/1995</t>
         </is>
       </c>
     </row>
@@ -1054,25 +1054,25 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Michael Mullins</t>
+          <t>Alexis Caldwell</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Function-based secondary knowledgebase</t>
+          <t>Visionary scalable implementation</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>william06@gmail.com</t>
+          <t>gonzalezdavid@gmail.com</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>82730400</v>
+        <v>89251883</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>1997-03-17</t>
+          <t>23/02/1983</t>
         </is>
       </c>
     </row>
@@ -1082,25 +1082,25 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Spencer Patton</t>
+          <t>Kristy Cole</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Horizontal system-worthy moratorium</t>
+          <t>Distributed actuating productivity</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>banthony@yahoo.com</t>
+          <t>russelldennis@walton.com</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>84531716</v>
+        <v>89483786</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>1996-05-12</t>
+          <t>11/05/1988</t>
         </is>
       </c>
     </row>
@@ -1110,25 +1110,25 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Stacey Morales</t>
+          <t>Teresa Kelly</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Mandatory analyzing toolset</t>
+          <t>Intuitive executive open architecture</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>younglisa@yahoo.com</t>
+          <t>david23@hotmail.com</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>83113324</v>
+        <v>82731976</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2000-07-25</t>
+          <t>20/09/2011</t>
         </is>
       </c>
     </row>
@@ -1138,25 +1138,25 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Joe Salas</t>
+          <t>Samuel Turner</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Focused 3rdgeneration budgetary management</t>
+          <t>Implemented user-facing implementation</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>austin52@alvarez.org</t>
+          <t>ryanbrooks@chambers.net</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>81700451</v>
+        <v>84032601</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2000-02-08</t>
+          <t>10/05/2008</t>
         </is>
       </c>
     </row>
@@ -1166,25 +1166,25 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Gregory Brooks</t>
+          <t>Mark Preston</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Inverse intermediate infrastructure</t>
+          <t>Right-sized zero tolerance protocol</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>joymartinez@baxter-harris.com</t>
+          <t>philiphawkins@hotmail.com</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>88422010</v>
+        <v>86987155</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2008-08-26</t>
+          <t>11/05/1973</t>
         </is>
       </c>
     </row>
@@ -1194,25 +1194,25 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Elizabeth Molina</t>
+          <t>Molly Shaw</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Front-line incremental concept</t>
+          <t>Networked maximized neural-net</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>samuelrobinson@gmail.com</t>
+          <t>davisdaniel@hotmail.com</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>82756313</v>
+        <v>88962069</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2001-10-29</t>
+          <t>18/05/2014</t>
         </is>
       </c>
     </row>
@@ -1222,25 +1222,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>William Sherman</t>
+          <t>Emily Hill</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Optimized encompassing challenge</t>
+          <t>Profit-focused actuating architecture</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>harperdiana@gmail.com</t>
+          <t>ymaldonado@garcia.com</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>84773518</v>
+        <v>86721027</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>1994-10-06</t>
+          <t>11/08/2001</t>
         </is>
       </c>
     </row>
@@ -1250,25 +1250,25 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Eric Holland</t>
+          <t>Helen Carter</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Devolved non-volatile access</t>
+          <t>Multi-lateral empowering approach</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ortizsabrina@hotmail.com</t>
+          <t>frank73@hotmail.com</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>88980510</v>
+        <v>80823008</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>1978-04-08</t>
+          <t>08/08/2013</t>
         </is>
       </c>
     </row>
@@ -1278,25 +1278,25 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Andrew Hess</t>
+          <t>Jeffrey Griffin</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Distributed zero-defect parallelism</t>
+          <t>Synergized 24/7 alliance</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>hyang@mccoy-scott.com</t>
+          <t>marquezdawn@gmail.com</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>89785799</v>
+        <v>82828942</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>1982-07-12</t>
+          <t>11/01/1989</t>
         </is>
       </c>
     </row>
@@ -1306,25 +1306,25 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Tyler Moyer</t>
+          <t>Luis Austin</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Distributed foreground benchmark</t>
+          <t>Re-engineered context-sensitive budgetary management</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>fordphillip@hotmail.com</t>
+          <t>emmabradshaw@lee.com</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>88490408</v>
+        <v>80342860</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2013-02-24</t>
+          <t>15/01/2005</t>
         </is>
       </c>
     </row>
@@ -1334,25 +1334,25 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Andrew Wagner</t>
+          <t>Heather Allen</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Inverse client-server architecture</t>
+          <t>Cross-group composite utilization</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>jonathanstevens@howard.com</t>
+          <t>lopezjohn@hinton.com</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>80337078</v>
+        <v>88471055</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>1981-02-05</t>
+          <t>18/04/1999</t>
         </is>
       </c>
     </row>
@@ -1362,25 +1362,25 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Kevin Harris</t>
+          <t>Monica Herring</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Optimized maximized Internet solution</t>
+          <t>Phased discrete attitude</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>ivan93@hotmail.com</t>
+          <t>evansricardo@gmail.com</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>83984383</v>
+        <v>84527699</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>1994-04-19</t>
+          <t>08/04/2002</t>
         </is>
       </c>
     </row>
@@ -1390,25 +1390,25 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Marie Page</t>
+          <t>Kristine Gallagher</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Business-focused uniform complexity</t>
+          <t>Realigned needs-based core</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>psanchez@hansen.biz</t>
+          <t>wsellers@yahoo.com</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>80637790</v>
+        <v>84817636</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>1991-06-27</t>
+          <t>28/11/2015</t>
         </is>
       </c>
     </row>
@@ -1418,25 +1418,25 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Brian Massey</t>
+          <t>Erika Bush</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>De-engineered empowering conglomeration</t>
+          <t>Balanced multimedia Graphical User Interface</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>schneiderchristian@brown.com</t>
+          <t>monique76@hotmail.com</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>86925208</v>
+        <v>81601655</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>1984-09-15</t>
+          <t>15/05/1984</t>
         </is>
       </c>
     </row>
@@ -1446,25 +1446,25 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Richard Cruz</t>
+          <t>Judy Rich</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Business-focused secondary customer loyalty</t>
+          <t>Synchronized dynamic standardization</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>kchavez@yahoo.com</t>
+          <t>leonsmith@yahoo.com</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>87164449</v>
+        <v>81737666</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>1973-04-29</t>
+          <t>14/11/2009</t>
         </is>
       </c>
     </row>
@@ -1474,25 +1474,25 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Oscar Aguirre</t>
+          <t>Richard Johnson</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Adaptive system-worthy analyzer</t>
+          <t>Customer-focused asynchronous flexibility</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>kenneth30@gmail.com</t>
+          <t>andersonjacob@lawson-santos.com</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>84020768</v>
+        <v>89697007</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2019-05-01</t>
+          <t>03/10/2009</t>
         </is>
       </c>
     </row>
@@ -1502,25 +1502,25 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Tony Curry</t>
+          <t>Alyssa Patterson</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Right-sized upward-trending solution</t>
+          <t>Total neutral algorithm</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>gyork@gmail.com</t>
+          <t>vhunter@flores.org</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>82239321</v>
+        <v>81461623</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2020-03-30</t>
+          <t>20/03/1993</t>
         </is>
       </c>
     </row>
@@ -1530,25 +1530,25 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Antonio Simmons</t>
+          <t>Caitlin Bradley</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Compatible dedicated initiative</t>
+          <t>Open-source motivating paradigm</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>justincollins@gmail.com</t>
+          <t>hnguyen@williams.com</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>86127068</v>
+        <v>84505626</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2016-09-16</t>
+          <t>28/04/2001</t>
         </is>
       </c>
     </row>
@@ -1558,25 +1558,25 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Joanne Gonzalez</t>
+          <t>Jason Moody</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Grass-roots 24/7 collaboration</t>
+          <t>Managed homogeneous adapter</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>william54@munoz.com</t>
+          <t>bishopbriana@howard.com</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>83305693</v>
+        <v>86440805</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2020-03-07</t>
+          <t>28/10/1993</t>
         </is>
       </c>
     </row>
@@ -1586,25 +1586,25 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Gregory Ross</t>
+          <t>Austin Logan</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>De-engineered optimizing Local Area Network</t>
+          <t>Function-based cohesive firmware</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>pearsonwanda@brown.com</t>
+          <t>katherinebooker@long.com</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>88007193</v>
+        <v>83720405</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>1972-03-22</t>
+          <t>06/10/1973</t>
         </is>
       </c>
     </row>
@@ -1614,25 +1614,25 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Angelica Oneill</t>
+          <t>Nicole Wood</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Fully-configurable tertiary success</t>
+          <t>Team-oriented responsive Local Area Network</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>michaelwhitaker@khan-james.org</t>
+          <t>glovercurtis@yahoo.com</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>89290733</v>
+        <v>80115673</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>1989-09-10</t>
+          <t>22/06/1981</t>
         </is>
       </c>
     </row>
@@ -1642,25 +1642,25 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>David Simon</t>
+          <t>Nicole Vaughn</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Front-line context-sensitive conglomeration</t>
+          <t>Assimilated exuding toolset</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>jcosta@walker-beck.biz</t>
+          <t>theresasmith@montes.com</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>88537748</v>
+        <v>80158509</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>1988-02-09</t>
+          <t>10/12/1973</t>
         </is>
       </c>
     </row>
@@ -1670,25 +1670,25 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Tara Dickerson</t>
+          <t>Thomas Bowman</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Ameliorated next generation Internet solution</t>
+          <t>Open-source actuating implementation</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>vanessa75@hogan.biz</t>
+          <t>clarkkatie@jackson.com</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>88214889</v>
+        <v>84481640</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>1978-02-22</t>
+          <t>17/05/1986</t>
         </is>
       </c>
     </row>
@@ -1698,25 +1698,25 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Gregory Nolan</t>
+          <t>Jessica Thomas DDS</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Versatile high-level frame</t>
+          <t>User-friendly bi-directional methodology</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>skinnertyrone@gmail.com</t>
+          <t>jennifer04@hotmail.com</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>88073284</v>
+        <v>88056842</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2011-08-18</t>
+          <t>01/09/1986</t>
         </is>
       </c>
     </row>
@@ -1726,25 +1726,25 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Jonathan Porter</t>
+          <t>Kevin Smith</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Polarized cohesive model</t>
+          <t>Robust secondary algorithm</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>hharvey@yahoo.com</t>
+          <t>jrobbins@hernandez-mccoy.com</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>85829170</v>
+        <v>83267772</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>1975-11-28</t>
+          <t>28/10/1977</t>
         </is>
       </c>
     </row>
@@ -1754,25 +1754,25 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Ronald Kelly</t>
+          <t>Sandra Gomez</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Synchronized directional moratorium</t>
+          <t>Open-source heuristic concept</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>hmeyer@wright-hanson.net</t>
+          <t>dorothy30@jackson-aguilar.info</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>85765126</v>
+        <v>81142560</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2009-10-31</t>
+          <t>20/10/2005</t>
         </is>
       </c>
     </row>
@@ -1782,25 +1782,25 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Ethan Smith</t>
+          <t>Edward Decker</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Face-to-face even-keeled projection</t>
+          <t>Balanced executive Graphic Interface</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>jenniferwatts@larsen.com</t>
+          <t>kevin16@daniels.com</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>89823461</v>
+        <v>85172182</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1983-01-10</t>
+          <t>17/02/2007</t>
         </is>
       </c>
     </row>
@@ -1810,25 +1810,25 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Daniel Smith</t>
+          <t>Christopher Gomez</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Diverse discrete alliance</t>
+          <t>Business-focused zero-defect flexibility</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>estein@schultz-hart.com</t>
+          <t>jonathanandrews@bond.com</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>86502224</v>
+        <v>83420116</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2003-05-02</t>
+          <t>03/05/1990</t>
         </is>
       </c>
     </row>
@@ -1838,25 +1838,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Matthew Johnson</t>
+          <t>John Wells</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Programmable background encryption</t>
+          <t>Quality-focused multi-tasking algorithm</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>waltonstephanie@dennis-smith.com</t>
+          <t>icrawford@pierce.com</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>81243402</v>
+        <v>82056244</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2019-11-22</t>
+          <t>02/07/2010</t>
         </is>
       </c>
     </row>
@@ -1866,25 +1866,25 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Mrs. Laura Crawford MD</t>
+          <t>Emily Schmitt</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Virtual didactic productivity</t>
+          <t>Self-enabling asymmetric task-force</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>joshuagarcia@hotmail.com</t>
+          <t>samuelmolina@rhodes-wright.com</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>84009828</v>
+        <v>83011471</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>1977-12-01</t>
+          <t>25/09/2003</t>
         </is>
       </c>
     </row>
@@ -1894,25 +1894,25 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Alicia Brown</t>
+          <t>Michelle Johnson</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Cross-group 6thgeneration synergy</t>
+          <t>Streamlined dedicated open system</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>scott47@hotmail.com</t>
+          <t>lorireynolds@bennett.net</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>80767453</v>
+        <v>86964109</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>1984-05-13</t>
+          <t>20/12/2008</t>
         </is>
       </c>
     </row>
@@ -1922,25 +1922,25 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Jacob Gordon</t>
+          <t>Dwayne Bonilla</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Organic real-time Local Area Network</t>
+          <t>User-friendly neutral software</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>maria16@hotmail.com</t>
+          <t>christianlang@gmail.com</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>89580617</v>
+        <v>88780353</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2018-09-01</t>
+          <t>11/01/1992</t>
         </is>
       </c>
     </row>
@@ -1950,25 +1950,25 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Daniel Davis</t>
+          <t>Ashley Johnson</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Profit-focused intermediate approach</t>
+          <t>Phased client-server task-force</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>bmartin@gmail.com</t>
+          <t>adamdelgado@yahoo.com</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>84110653</v>
+        <v>84361100</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2018-01-19</t>
+          <t>31/12/1993</t>
         </is>
       </c>
     </row>
@@ -1978,25 +1978,25 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>David Williams</t>
+          <t>Brian Hobbs</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Re-engineered uniform collaboration</t>
+          <t>Focused radical adapter</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>greenjoseph@yahoo.com</t>
+          <t>alexander45@nguyen.info</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>89447095</v>
+        <v>82327083</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>1998-08-02</t>
+          <t>17/06/2011</t>
         </is>
       </c>
     </row>
@@ -2006,25 +2006,25 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Ruben Ortiz</t>
+          <t>Mark Carpenter</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Upgradable value-added analyzer</t>
+          <t>Total scalable capacity</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>daniel42@hotmail.com</t>
+          <t>hicksmary@yahoo.com</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>80373806</v>
+        <v>81190046</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>1980-02-16</t>
+          <t>06/03/1974</t>
         </is>
       </c>
     </row>
@@ -2034,25 +2034,25 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Teresa Parker</t>
+          <t>Brittany Gonzalez</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Cross-platform object-oriented moratorium</t>
+          <t>Right-sized global hub</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>travistownsend@davis.com</t>
+          <t>dyoung@anderson-zimmerman.net</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>86886231</v>
+        <v>82018479</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>1996-05-23</t>
+          <t>08/01/2007</t>
         </is>
       </c>
     </row>
@@ -2062,25 +2062,25 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Robin Cruz</t>
+          <t>Jamie Fowler</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Horizontal uniform knowledgebase</t>
+          <t>Enterprise-wide bottom-line functionalities</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>william10@yahoo.com</t>
+          <t>gutierrezaaron@valencia.com</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>81725682</v>
+        <v>86942532</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>2012-05-29</t>
+          <t>01/05/1991</t>
         </is>
       </c>
     </row>
@@ -2090,25 +2090,25 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Heather Jackson</t>
+          <t>Craig Rogers</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Business-focused needs-based contingency</t>
+          <t>Sharable tangible pricing structure</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>lancemarsh@hotmail.com</t>
+          <t>moorejoseph@hotmail.com</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>88491072</v>
+        <v>89398934</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2003-09-13</t>
+          <t>05/01/1978</t>
         </is>
       </c>
     </row>
@@ -2118,25 +2118,25 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>John Moore</t>
+          <t>Mrs. Lauren Beard DDS</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Visionary regional core</t>
+          <t>Secured empowering moratorium</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>benjaminsmith@gmail.com</t>
+          <t>wardtracy@hotmail.com</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>83393898</v>
+        <v>87372546</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>2000-01-19</t>
+          <t>06/03/1971</t>
         </is>
       </c>
     </row>
@@ -2146,25 +2146,25 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Steven Houston</t>
+          <t>Nancy Davis</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Up-sized foreground data-warehouse</t>
+          <t>Polarized background archive</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>tsanchez@gmail.com</t>
+          <t>reedbeth@hotmail.com</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>81807617</v>
+        <v>83026827</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>1999-07-29</t>
+          <t>15/01/2014</t>
         </is>
       </c>
     </row>
@@ -2174,25 +2174,25 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Richard Randolph</t>
+          <t>Abigail Yang</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Centralized clear-thinking system engine</t>
+          <t>Phased actuating productivity</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>sydney81@hill-myers.org</t>
+          <t>hjohnson@myers.info</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>87655720</v>
+        <v>88018040</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>2002-10-06</t>
+          <t>03/11/2000</t>
         </is>
       </c>
     </row>
@@ -2202,25 +2202,25 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Brian Lawrence</t>
+          <t>Teresa Morales</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Enterprise-wide homogeneous groupware</t>
+          <t>Phased client-server matrix</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>ruth09@yahoo.com</t>
+          <t>ralvarez@martinez.info</t>
         </is>
       </c>
       <c r="E64" t="n">
-        <v>89710077</v>
+        <v>86597197</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>1995-07-16</t>
+          <t>27/01/1978</t>
         </is>
       </c>
     </row>
@@ -2230,25 +2230,25 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Nicole Mccormick</t>
+          <t>Nathan Johnson</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Open-source static leverage</t>
+          <t>Face-to-face holistic time-frame</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>tashachristensen@gmail.com</t>
+          <t>collinstara@yahoo.com</t>
         </is>
       </c>
       <c r="E65" t="n">
-        <v>82343031</v>
+        <v>80321301</v>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>1974-10-09</t>
+          <t>23/07/1989</t>
         </is>
       </c>
     </row>
@@ -2258,25 +2258,25 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Mark Hall</t>
+          <t>Christopher Williams</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Phased stable solution</t>
+          <t>Object-based solution-oriented concept</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>brandismall@griffith.com</t>
+          <t>harrisjeffery@hotmail.com</t>
         </is>
       </c>
       <c r="E66" t="n">
-        <v>87556057</v>
+        <v>82076804</v>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>1995-05-26</t>
+          <t>16/01/2019</t>
         </is>
       </c>
     </row>
@@ -2286,25 +2286,25 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Mrs. Stephanie Nguyen DDS</t>
+          <t>Kimberly Green</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Customer-focused background alliance</t>
+          <t>Multi-lateral scalable matrix</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>jacobmitchell@harmon-taylor.net</t>
+          <t>hfisher@ortega-thomas.com</t>
         </is>
       </c>
       <c r="E67" t="n">
-        <v>82564783</v>
+        <v>87290113</v>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>1972-04-04</t>
+          <t>06/01/1997</t>
         </is>
       </c>
     </row>
@@ -2314,25 +2314,25 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Julia Jackson</t>
+          <t>Caroline Harrison</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Programmable 24hour superstructure</t>
+          <t>Grass-roots grid-enabled function</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>imiller@gmail.com</t>
+          <t>thompsonmichelle@quinn.biz</t>
         </is>
       </c>
       <c r="E68" t="n">
-        <v>85982182</v>
+        <v>87203679</v>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>2002-03-16</t>
+          <t>19/03/1974</t>
         </is>
       </c>
     </row>
@@ -2342,25 +2342,25 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Jeffrey Ortiz</t>
+          <t>Sonya Sanchez</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Advanced interactive frame</t>
+          <t>Realigned local task-force</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>aaron87@rivera-allen.com</t>
+          <t>morgan65@mclean.info</t>
         </is>
       </c>
       <c r="E69" t="n">
-        <v>83463626</v>
+        <v>80946112</v>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>1985-06-04</t>
+          <t>13/09/1971</t>
         </is>
       </c>
     </row>
@@ -2370,25 +2370,25 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Joseph Mckinney</t>
+          <t>Dale Rhodes</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Robust stable success</t>
+          <t>Organic content-based success</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>ronaldbarrera@hotmail.com</t>
+          <t>andrewsmatthew@hotmail.com</t>
         </is>
       </c>
       <c r="E70" t="n">
-        <v>85467668</v>
+        <v>83923608</v>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>1972-09-09</t>
+          <t>09/11/1989</t>
         </is>
       </c>
     </row>
@@ -2398,25 +2398,25 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>John Brown</t>
+          <t>Krystal Johnston</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Expanded multimedia conglomeration</t>
+          <t>Cross-group high-level approach</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>todd48@perez.com</t>
+          <t>ashley33@lewis.biz</t>
         </is>
       </c>
       <c r="E71" t="n">
-        <v>88177045</v>
+        <v>86587178</v>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>1992-08-30</t>
+          <t>06/07/2006</t>
         </is>
       </c>
     </row>
@@ -2426,25 +2426,25 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Paul Williams</t>
+          <t>Alexander Baldwin</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Future-proofed client-server model</t>
+          <t>Synchronized attitude-oriented Local Area Network</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>williamsalas@yahoo.com</t>
+          <t>ianwyatt@thomas.net</t>
         </is>
       </c>
       <c r="E72" t="n">
-        <v>83007331</v>
+        <v>84436096</v>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>1993-03-13</t>
+          <t>15/03/1993</t>
         </is>
       </c>
     </row>
@@ -2454,25 +2454,25 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Kaitlyn Williams</t>
+          <t>Randall Moore</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Vision-oriented client-driven function</t>
+          <t>Profit-focused executive function</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>emily30@jackson-watkins.org</t>
+          <t>grantjeffrey@gmail.com</t>
         </is>
       </c>
       <c r="E73" t="n">
-        <v>80330422</v>
+        <v>86588586</v>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>2006-01-10</t>
+          <t>06/04/1975</t>
         </is>
       </c>
     </row>
@@ -2482,25 +2482,25 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Corey Oconnell</t>
+          <t>Melvin Castro</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Reduced holistic neural-net</t>
+          <t>Configurable holistic hierarchy</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>morrisonrobert@james-fowler.org</t>
+          <t>doylerichard@yahoo.com</t>
         </is>
       </c>
       <c r="E74" t="n">
-        <v>82153349</v>
+        <v>80496035</v>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>1985-12-25</t>
+          <t>11/06/1980</t>
         </is>
       </c>
     </row>
@@ -2510,25 +2510,25 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Julie Carter</t>
+          <t>Melanie Atkins</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Enhanced discrete help-desk</t>
+          <t>Visionary reciprocal access</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>pwoods@gmail.com</t>
+          <t>amosley@stewart-james.com</t>
         </is>
       </c>
       <c r="E75" t="n">
-        <v>89710454</v>
+        <v>85244856</v>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>2000-04-04</t>
+          <t>25/07/1972</t>
         </is>
       </c>
     </row>
@@ -2538,25 +2538,25 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Kelly Finley</t>
+          <t>Mr. Robert Lewis MD</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Progressive 5thgeneration support</t>
+          <t>Upgradable needs-based secured line</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>laura15@nguyen.info</t>
+          <t>reynoldsrandall@zimmerman.com</t>
         </is>
       </c>
       <c r="E76" t="n">
-        <v>85177509</v>
+        <v>80865997</v>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>2009-01-13</t>
+          <t>23/04/1992</t>
         </is>
       </c>
     </row>
@@ -2566,25 +2566,25 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>David Kennedy</t>
+          <t>Elizabeth Marshall</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Total regional superstructure</t>
+          <t>Down-sized grid-enabled analyzer</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>ronaldfuentes@yahoo.com</t>
+          <t>garciabrandon@yahoo.com</t>
         </is>
       </c>
       <c r="E77" t="n">
-        <v>84510460</v>
+        <v>89717719</v>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>2007-06-06</t>
+          <t>09/08/2015</t>
         </is>
       </c>
     </row>
@@ -2594,25 +2594,25 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Michael Rivera</t>
+          <t>Michael Perez</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Ameliorated needs-based info-mediaries</t>
+          <t>Innovative responsive artificial intelligence</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>jenniferanthony@chavez.com</t>
+          <t>thompsonanthony@gmail.com</t>
         </is>
       </c>
       <c r="E78" t="n">
-        <v>84008880</v>
+        <v>87866388</v>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>1985-06-20</t>
+          <t>08/05/1976</t>
         </is>
       </c>
     </row>
@@ -2622,25 +2622,25 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Caleb Sanders</t>
+          <t>Kayla Martin</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Configurable interactive hub</t>
+          <t>Decentralized tertiary hub</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>cturner@smith.net</t>
+          <t>abigailvasquez@gmail.com</t>
         </is>
       </c>
       <c r="E79" t="n">
-        <v>86362051</v>
+        <v>83327937</v>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>2021-03-11</t>
+          <t>07/07/2008</t>
         </is>
       </c>
     </row>
@@ -2650,25 +2650,25 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Franklin Howard</t>
+          <t>Christopher Kim</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Stand-alone asymmetric policy</t>
+          <t>Streamlined tertiary task-force</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>vanessafletcher@rodriguez-alvarez.com</t>
+          <t>paul99@gmail.com</t>
         </is>
       </c>
       <c r="E80" t="n">
-        <v>86809080</v>
+        <v>86192166</v>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>1996-05-22</t>
+          <t>04/12/2005</t>
         </is>
       </c>
     </row>
@@ -2678,25 +2678,25 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Melanie Boyd</t>
+          <t>Gabrielle Hernandez</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Reverse-engineered web-enabled task-force</t>
+          <t>Optional bi-directional functionalities</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>carrollcarlos@hotmail.com</t>
+          <t>nicolehernandez@burnett-hernandez.com</t>
         </is>
       </c>
       <c r="E81" t="n">
-        <v>84528433</v>
+        <v>87219797</v>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>1978-09-29</t>
+          <t>24/04/2002</t>
         </is>
       </c>
     </row>
@@ -2706,25 +2706,25 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Hannah House</t>
+          <t>Timothy Clayton</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Multi-layered clear-thinking project</t>
+          <t>Down-sized discrete functionalities</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>elizabethhoffman@cook-rosales.com</t>
+          <t>along@watson-clark.com</t>
         </is>
       </c>
       <c r="E82" t="n">
-        <v>82820102</v>
+        <v>80760555</v>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>1998-01-09</t>
+          <t>31/05/2004</t>
         </is>
       </c>
     </row>
@@ -2734,25 +2734,25 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Shannon Garcia</t>
+          <t>Michelle Hoover</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Multi-layered exuding policy</t>
+          <t>Face-to-face bottom-line hub</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>rogersheather@gmail.com</t>
+          <t>bmolina@gmail.com</t>
         </is>
       </c>
       <c r="E83" t="n">
-        <v>83468254</v>
+        <v>81938019</v>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>2011-08-28</t>
+          <t>02/09/2013</t>
         </is>
       </c>
     </row>
@@ -2762,25 +2762,25 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Eric Green</t>
+          <t>Nicole Chang</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Reduced homogeneous definition</t>
+          <t>De-engineered mission-critical utilization</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>joyparker@yahoo.com</t>
+          <t>dustinlittle@kennedy.com</t>
         </is>
       </c>
       <c r="E84" t="n">
-        <v>81005193</v>
+        <v>83960814</v>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>2016-12-22</t>
+          <t>04/07/2013</t>
         </is>
       </c>
     </row>
@@ -2790,25 +2790,25 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Connie Nguyen</t>
+          <t>Dr. Andrea Knight</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Robust encompassing concept</t>
+          <t>Distributed next generation standardization</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>sherry76@gmail.com</t>
+          <t>blanchardstephen@carpenter.com</t>
         </is>
       </c>
       <c r="E85" t="n">
-        <v>84994539</v>
+        <v>86166411</v>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>1989-02-15</t>
+          <t>07/04/2018</t>
         </is>
       </c>
     </row>
@@ -2818,25 +2818,25 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Philip Burgess</t>
+          <t>Sandra Perez</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Down-sized well-modulated analyzer</t>
+          <t>Future-proofed asynchronous productivity</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>abigail00@erickson-hill.net</t>
+          <t>rcannon@barnes-morris.com</t>
         </is>
       </c>
       <c r="E86" t="n">
-        <v>88050451</v>
+        <v>82846545</v>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>2010-02-17</t>
+          <t>22/09/2015</t>
         </is>
       </c>
     </row>
@@ -2846,25 +2846,25 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Elizabeth Garcia</t>
+          <t>Dale Maldonado</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Grass-roots interactive benchmark</t>
+          <t>Fully-configurable 3rdgeneration middleware</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>morganjesus@hotmail.com</t>
+          <t>maria91@yahoo.com</t>
         </is>
       </c>
       <c r="E87" t="n">
-        <v>89605281</v>
+        <v>89148544</v>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>1997-09-28</t>
+          <t>20/02/2006</t>
         </is>
       </c>
     </row>
@@ -2874,25 +2874,25 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Katelyn Carlson</t>
+          <t>Kyle Williams</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Switchable eco-centric utilization</t>
+          <t>Digitized dedicated instruction set</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>cynthiawebster@leblanc.org</t>
+          <t>harveywayne@ortega-gonzales.com</t>
         </is>
       </c>
       <c r="E88" t="n">
-        <v>87198290</v>
+        <v>89982999</v>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>1976-06-27</t>
+          <t>02/06/1984</t>
         </is>
       </c>
     </row>
@@ -2902,25 +2902,25 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Terry Rice</t>
+          <t>Michael Deleon</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Fully-configurable incremental process improvement</t>
+          <t>Secured explicit standardization</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>barbara34@yahoo.com</t>
+          <t>melvinjackson@smith.net</t>
         </is>
       </c>
       <c r="E89" t="n">
-        <v>89330055</v>
+        <v>84340526</v>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>2000-02-02</t>
+          <t>31/01/1979</t>
         </is>
       </c>
     </row>
@@ -2930,25 +2930,25 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Amy Smith</t>
+          <t>Kathy Miller</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Profound contextually-based paradigm</t>
+          <t>Organized next generation benchmark</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>fitzpatrickryan@hotmail.com</t>
+          <t>monica70@gmail.com</t>
         </is>
       </c>
       <c r="E90" t="n">
-        <v>82552407</v>
+        <v>83456190</v>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>2001-06-22</t>
+          <t>20/03/1996</t>
         </is>
       </c>
     </row>
@@ -2958,25 +2958,25 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Heather Harris</t>
+          <t>Nathaniel Williamson</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Streamlined foreground function</t>
+          <t>Assimilated human-resource throughput</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>brandongarcia@hotmail.com</t>
+          <t>rsmith@yahoo.com</t>
         </is>
       </c>
       <c r="E91" t="n">
-        <v>82552313</v>
+        <v>81816072</v>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>1992-10-23</t>
+          <t>31/07/2004</t>
         </is>
       </c>
     </row>
@@ -2986,25 +2986,25 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Tyler Mullins</t>
+          <t>Jeffrey Butler</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Stand-alone content-based interface</t>
+          <t>Down-sized global help-desk</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>gentryjennifer@wilson-moore.net</t>
+          <t>edwardssharon@hotmail.com</t>
         </is>
       </c>
       <c r="E92" t="n">
-        <v>82143096</v>
+        <v>86302188</v>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>1976-06-27</t>
+          <t>12/10/2012</t>
         </is>
       </c>
     </row>
@@ -3014,25 +3014,25 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Russell Phillips</t>
+          <t>Laura Gonzales</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Multi-lateral needs-based leverage</t>
+          <t>Optimized asynchronous flexibility</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>kpace@hotmail.com</t>
+          <t>tommy33@howard.net</t>
         </is>
       </c>
       <c r="E93" t="n">
-        <v>82582677</v>
+        <v>84756019</v>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>2005-05-24</t>
+          <t>24/04/1978</t>
         </is>
       </c>
     </row>
@@ -3042,25 +3042,25 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>James Mora</t>
+          <t>Erica Durham</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Secured regional core</t>
+          <t>Open-architected solution-oriented customer loyalty</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>amacdonald@yahoo.com</t>
+          <t>rebecca74@yahoo.com</t>
         </is>
       </c>
       <c r="E94" t="n">
-        <v>86962142</v>
+        <v>81671730</v>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>2003-09-26</t>
+          <t>12/02/2006</t>
         </is>
       </c>
     </row>
@@ -3070,25 +3070,25 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Lauren Schaefer</t>
+          <t>Eric White</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Down-sized tangible software</t>
+          <t>Centralized non-volatile contingency</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>jeffreyball@newman.com</t>
+          <t>salazarjennifer@hotmail.com</t>
         </is>
       </c>
       <c r="E95" t="n">
-        <v>85186243</v>
+        <v>82693084</v>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>2015-12-29</t>
+          <t>11/04/1982</t>
         </is>
       </c>
     </row>
@@ -3098,25 +3098,25 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Julie Aguirre</t>
+          <t>Stephanie Barnes</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Expanded systematic Graphic Interface</t>
+          <t>Extended foreground emulation</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>gwhite@hughes-johnson.net</t>
+          <t>stephaniegray@yahoo.com</t>
         </is>
       </c>
       <c r="E96" t="n">
-        <v>80331365</v>
+        <v>86637283</v>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>2005-11-04</t>
+          <t>03/11/1995</t>
         </is>
       </c>
     </row>
@@ -3126,25 +3126,25 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Jeanne Robbins</t>
+          <t>Patrick Shaw</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Adaptive motivating hub</t>
+          <t>Digitized intermediate Internet solution</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>alexlucero@ball-harris.info</t>
+          <t>lucasshelley@martin.com</t>
         </is>
       </c>
       <c r="E97" t="n">
-        <v>82736367</v>
+        <v>88906148</v>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>1985-07-21</t>
+          <t>21/05/2016</t>
         </is>
       </c>
     </row>
@@ -3154,25 +3154,25 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Kayla Fry</t>
+          <t>Keith Williams</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Secured eco-centric Graphical User Interface</t>
+          <t>Virtual tertiary capability</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>heather07@hotmail.com</t>
+          <t>kennethharrison@hayes.com</t>
         </is>
       </c>
       <c r="E98" t="n">
-        <v>85751304</v>
+        <v>85494213</v>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>1990-08-05</t>
+          <t>12/06/1980</t>
         </is>
       </c>
     </row>
@@ -3182,25 +3182,25 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Allen Moreno</t>
+          <t>Eric Johnson</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Versatile client-driven challenge</t>
+          <t>Quality-focused client-driven database</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>wesleywatson@thomas.biz</t>
+          <t>pauljones@yahoo.com</t>
         </is>
       </c>
       <c r="E99" t="n">
-        <v>85004834</v>
+        <v>83730774</v>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>2019-05-16</t>
+          <t>04/05/1999</t>
         </is>
       </c>
     </row>
@@ -3210,25 +3210,25 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Michael Levy</t>
+          <t>Sarah Carter DDS</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Multi-layered asymmetric open architecture</t>
+          <t>Innovative fresh-thinking parallelism</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>winterskelly@barnett.com</t>
+          <t>mccartyjack@gmail.com</t>
         </is>
       </c>
       <c r="E100" t="n">
-        <v>80066091</v>
+        <v>83777921</v>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>1980-12-31</t>
+          <t>11/06/1974</t>
         </is>
       </c>
     </row>
@@ -3238,25 +3238,25 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Kara Glenn</t>
+          <t>Ashley Ross</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Realigned incremental budgetary management</t>
+          <t>Re-engineered upward-trending superstructure</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>boydnancy@hotmail.com</t>
+          <t>pamelagoodman@gmail.com</t>
         </is>
       </c>
       <c r="E101" t="n">
-        <v>83845151</v>
+        <v>88718161</v>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>2006-02-26</t>
+          <t>12/02/1991</t>
         </is>
       </c>
     </row>

</xml_diff>